<commit_message>
last few airbnb classes
</commit_message>
<xml_diff>
--- a/com.airbnb/src/test/resources/TestData.xlsx
+++ b/com.airbnb/src/test/resources/TestData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erdosa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erdosa\IdeaProjects\Selenium_Framework_Team2\com.airbnb\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7AC84BA-F3B4-4DB5-ABB3-48E169491698}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5687C9-F482-4ED7-A94C-6C8C4074124F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E8A104B-F2B9-46B0-BA3D-725330091B04}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{2E8A104B-F2B9-46B0-BA3D-725330091B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Languages" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidPhoneErrorMessage" sheetId="2" r:id="rId2"/>
+    <sheet name="Inspiration Getaways" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,31 +27,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>English\nUnited States</t>
-  </si>
-  <si>
-    <t>Azərbaycan dili\nAzərbaycan</t>
-  </si>
-  <si>
-    <t>Bahasa Indonesia\nIndonesia</t>
-  </si>
-  <si>
-    <t>Bosanski\nBosna i Hercegovina</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Bahasa Indonesia
+Indonesia</t>
+  </si>
+  <si>
+    <t>English
+United States</t>
+  </si>
+  <si>
+    <t>You'll need to use a different phone number, we can't support this one1.</t>
+  </si>
+  <si>
+    <t>Bosanski1
+Bosna i Hercegovina</t>
+  </si>
+  <si>
+    <t>Azərbaycan dili1
+Azərbaycan</t>
+  </si>
+  <si>
+    <t>Destinations for arts &amp; culture</t>
+  </si>
+  <si>
+    <t>Destinations for outdoor adventure</t>
+  </si>
+  <si>
+    <t>Mountain cabins</t>
+  </si>
+  <si>
+    <t>Beach destinations</t>
+  </si>
+  <si>
+    <t>Popular destinations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,8 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,34 +424,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CAD258-5442-467F-B87C-F9011B753ADF}">
   <dimension ref="A1:A4"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2ACDD36-2169-47BA-A90E-4B01DD7C213C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B926F9-9305-480E-B347-7756122DE437}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expedia few more test cases
</commit_message>
<xml_diff>
--- a/com.airbnb/src/test/resources/TestData.xlsx
+++ b/com.airbnb/src/test/resources/TestData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erdosa\IdeaProjects\Selenium_Framework_Team2\com.airbnb\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5687C9-F482-4ED7-A94C-6C8C4074124F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C10B187-4A79-4420-BDA1-D18598F5F0FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{2E8A104B-F2B9-46B0-BA3D-725330091B04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{2E8A104B-F2B9-46B0-BA3D-725330091B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Languages" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidPhoneErrorMessage" sheetId="2" r:id="rId2"/>
     <sheet name="Inspiration Getaways" sheetId="3" r:id="rId3"/>
+    <sheet name="Languages1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="141">
   <si>
     <t>Bahasa Indonesia
 Indonesia</t>
@@ -61,6 +62,408 @@
   </si>
   <si>
     <t>Popular destinations</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Eesti</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Belice</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>España</t>
+  </si>
+  <si>
+    <t>Estados Unidos</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Latinoamérica</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Panamá</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Perú</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>Belgique</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Suisse</t>
+  </si>
+  <si>
+    <t>Gaeilge</t>
+  </si>
+  <si>
+    <t>Éire</t>
+  </si>
+  <si>
+    <t>Hrvatski</t>
+  </si>
+  <si>
+    <t>Hrvatska</t>
+  </si>
+  <si>
+    <t>isiXhosa</t>
+  </si>
+  <si>
+    <t>eMzantsi Afrika</t>
+  </si>
+  <si>
+    <t>isiZulu</t>
+  </si>
+  <si>
+    <t>iNingizimu Afrika</t>
+  </si>
+  <si>
+    <t>Íslenska</t>
+  </si>
+  <si>
+    <t>Ísland</t>
+  </si>
+  <si>
+    <t>Italiano</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Svizzera</t>
+  </si>
+  <si>
+    <t>Kiswahili</t>
+  </si>
+  <si>
+    <t>Āfrika</t>
+  </si>
+  <si>
+    <t>Latviešu</t>
+  </si>
+  <si>
+    <t>Latvija</t>
+  </si>
+  <si>
+    <t>Lietuvių</t>
+  </si>
+  <si>
+    <t>Lietuva</t>
+  </si>
+  <si>
+    <t>Magyar</t>
+  </si>
+  <si>
+    <t>Magyarország</t>
+  </si>
+  <si>
+    <t>Malti</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Melayu</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Nederlands</t>
+  </si>
+  <si>
+    <t>België</t>
+  </si>
+  <si>
+    <t>Nederland</t>
+  </si>
+  <si>
+    <t>Norsk</t>
+  </si>
+  <si>
+    <t>Norge</t>
+  </si>
+  <si>
+    <t>Polski</t>
+  </si>
+  <si>
+    <t>Polska</t>
+  </si>
+  <si>
+    <t>Português</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Română</t>
+  </si>
+  <si>
+    <t>România</t>
+  </si>
+  <si>
+    <t>Shqip</t>
+  </si>
+  <si>
+    <t>Shqipëri</t>
+  </si>
+  <si>
+    <t>Slovenčina</t>
+  </si>
+  <si>
+    <t>Slovensko</t>
+  </si>
+  <si>
+    <t>Slovenščina</t>
+  </si>
+  <si>
+    <t>Slovenija</t>
+  </si>
+  <si>
+    <t>Srpski</t>
+  </si>
+  <si>
+    <t>Srbija</t>
+  </si>
+  <si>
+    <t>Suomi</t>
+  </si>
+  <si>
+    <t>Svenska</t>
+  </si>
+  <si>
+    <t>Sverige</t>
+  </si>
+  <si>
+    <t>Tagalog</t>
+  </si>
+  <si>
+    <t>Pilipinas</t>
+  </si>
+  <si>
+    <t>Tiếng Việt</t>
+  </si>
+  <si>
+    <t>Việt Nam</t>
+  </si>
+  <si>
+    <t>Türkçe</t>
+  </si>
+  <si>
+    <t>Türkiye</t>
+  </si>
+  <si>
+    <t>Ελληνικά</t>
+  </si>
+  <si>
+    <t>Ελλάδα</t>
+  </si>
+  <si>
+    <t>Български</t>
+  </si>
+  <si>
+    <t>България</t>
+  </si>
+  <si>
+    <t>Македонски</t>
+  </si>
+  <si>
+    <t>Северна Македонија</t>
+  </si>
+  <si>
+    <t>Русский</t>
+  </si>
+  <si>
+    <t>Россия</t>
+  </si>
+  <si>
+    <t>Українська</t>
+  </si>
+  <si>
+    <t>Україна</t>
+  </si>
+  <si>
+    <t>ქართული</t>
+  </si>
+  <si>
+    <t>საქართველო</t>
+  </si>
+  <si>
+    <t>Հայերեն</t>
+  </si>
+  <si>
+    <t>Հայաստան</t>
+  </si>
+  <si>
+    <t>עברית</t>
+  </si>
+  <si>
+    <t>ישראל</t>
+  </si>
+  <si>
+    <t>العربية</t>
+  </si>
+  <si>
+    <t>العالم</t>
+  </si>
+  <si>
+    <t>हिन्दी</t>
+  </si>
+  <si>
+    <t>भारत</t>
+  </si>
+  <si>
+    <t>ไทย</t>
+  </si>
+  <si>
+    <t>ประเทศไทย</t>
+  </si>
+  <si>
+    <t>한국어</t>
+  </si>
+  <si>
+    <t>대한민국</t>
+  </si>
+  <si>
+    <t>日本語</t>
+  </si>
+  <si>
+    <t>日本</t>
+  </si>
+  <si>
+    <t>简体中文</t>
+  </si>
+  <si>
+    <t>美国</t>
+  </si>
+  <si>
+    <t>繁體中文</t>
+  </si>
+  <si>
+    <t>美國</t>
+  </si>
+  <si>
+    <t>中国</t>
+  </si>
+  <si>
+    <t>香港</t>
+  </si>
+  <si>
+    <t>台灣</t>
+  </si>
+  <si>
+    <t>Azərbaycan dili
+Azərbaycan</t>
+  </si>
+  <si>
+    <t>Bosanski
+Bosna i Hercegovina</t>
+  </si>
+  <si>
+    <t>Català
+Espanya</t>
+  </si>
+  <si>
+    <t>Čeština
+Česká republika</t>
+  </si>
+  <si>
+    <t>Crnogorski
+Crna Gora</t>
+  </si>
+  <si>
+    <t>Dansk
+Danmark</t>
+  </si>
+  <si>
+    <t>Deutsch
+Deutschland</t>
+  </si>
+  <si>
+    <t>Deutsch
+Österreich</t>
+  </si>
+  <si>
+    <t>Deutsch
+Schweiz</t>
   </si>
 </sst>
 </file>
@@ -482,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B926F9-9305-480E-B347-7756122DE437}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -516,4 +919,878 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92868405-E188-4E01-A4D0-3A7CE54B0011}">
+  <dimension ref="A1:A171"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>